<commit_message>
serial trigger reading codes
</commit_message>
<xml_diff>
--- a/Sepehr/fMRI/psychopy/loopTemplate18.xlsx
+++ b/Sepehr/fMRI/psychopy/loopTemplate18.xlsx
@@ -443,126 +443,126 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CCW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CCW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CCW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>./images2/Sphere_Ref_BG-grey_stim-yellow.png</t>
+          <t>./images_eeg/Sphere_CCW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CCW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_Ref_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CCW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CCW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CCW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_Ref_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>./images2/Sphere_Ref_BG-grey_stim-yellow.png</t>
+          <t>./images_eeg/Sphere_CCW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>./images2/Sphere_Ref_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_Ref_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CCW-3_BG-grey_stim-yellow.png</t>
+          <t>./images_eeg/Sphere_CW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CCW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CCW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>./images2/Sphere_Ref_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CCW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_Ref_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CW-3_BG-grey_stim-yellow.png</t>
+          <t>./images_eeg/Sphere_CCW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>./images2/Sphere_CW-3_BG-grey_stim-white.png</t>
+          <t>./images_eeg/Sphere_CW-3.75_BG-grey_stim-white.png</t>
         </is>
       </c>
     </row>

</xml_diff>